<commit_message>
Fix label in FORWARD AND BACKWARD and update regconv
</commit_message>
<xml_diff>
--- a/ref/reg convention.xlsx
+++ b/ref/reg convention.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>JR</t>
   </si>
@@ -69,6 +69,57 @@
   </si>
   <si>
     <t>tmp3</t>
+  </si>
+  <si>
+    <t>line color</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>tmp4</t>
+  </si>
+  <si>
+    <t>tmp5</t>
+  </si>
+  <si>
+    <t>tmp6</t>
+  </si>
+  <si>
+    <t>tmp7</t>
+  </si>
+  <si>
+    <t>tmp8</t>
+  </si>
+  <si>
+    <t>tmp9</t>
+  </si>
+  <si>
+    <t>tmp10</t>
+  </si>
+  <si>
+    <t>tmp11</t>
+  </si>
+  <si>
+    <t>pen down/up</t>
+  </si>
+  <si>
+    <t>DMEM stack ptr</t>
   </si>
 </sst>
 </file>
@@ -78,8 +129,16 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -187,12 +246,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -200,6 +258,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,265 +601,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:J28"/>
+  <dimension ref="E4:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E4" t="s">
+    <row r="4" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E4" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="5:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E6" s="2">
         <v>0</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="11">
         <v>0</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E7" s="5">
+      <c r="I6" s="2">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="12">
         <v>1</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E8" s="5">
+      <c r="I7" s="4">
+        <v>17</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="12">
         <v>2</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E9" s="5">
+      <c r="I8" s="4">
+        <v>18</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="13">
         <v>3</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E10" s="5">
+      <c r="I9" s="4">
+        <v>19</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5">
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="4">
         <v>20</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E11" s="5">
+      <c r="J10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E11" s="4">
         <v>5</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="5">
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="4">
         <v>21</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E12" s="5">
+      <c r="J11" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E12" s="4">
         <v>6</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="5">
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="4">
         <v>22</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E13" s="5">
+      <c r="J12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E13" s="4">
         <v>7</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="5">
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4">
         <v>23</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E14" s="5">
+      <c r="J13" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E14" s="4">
         <v>8</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="5">
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="4">
         <v>24</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E15" s="5">
+      <c r="J14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E15" s="4">
         <v>9</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="5">
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="4">
         <v>25</v>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E16" s="5">
+      <c r="J15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E16" s="4">
         <v>10</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="5">
+      <c r="G16" s="5"/>
+      <c r="H16" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="4">
         <v>26</v>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E17" s="5">
+      <c r="J16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E17" s="4">
         <v>11</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="5">
+      <c r="G17" s="5"/>
+      <c r="H17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="4">
         <v>27</v>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E18" s="5">
+      <c r="J17" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E18" s="4">
         <v>12</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5">
+      <c r="G18" s="5"/>
+      <c r="H18" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="4">
         <v>28</v>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E19" s="5">
+      <c r="J18" s="10"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E19" s="4">
         <v>13</v>
       </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="5">
+      <c r="F19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="4">
         <v>29</v>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E20" s="5">
+      <c r="J19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E20" s="4">
         <v>14</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="5">
+      <c r="F20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="4">
         <v>30</v>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="8">
+      <c r="J20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="21"/>
+    </row>
+    <row r="21" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="7">
         <v>15</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="8">
+      <c r="F21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8"/>
+      <c r="H21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="7">
         <v>31</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="J21" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J21" s="10"/>
-    </row>
-    <row r="22" spans="5:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="8"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E28" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix duplicate labels and add DMEM convention and registers
</commit_message>
<xml_diff>
--- a/ref/reg convention.xlsx
+++ b/ref/reg convention.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DMEM state " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>JR</t>
   </si>
@@ -120,6 +121,30 @@
   </si>
   <si>
     <t>DMEM stack ptr</t>
+  </si>
+  <si>
+    <t>DMEM State entry convention</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>pen color</t>
+  </si>
+  <si>
+    <t>orientation</t>
+  </si>
+  <si>
+    <t>turtle image index</t>
+  </si>
+  <si>
+    <t>Turtle image index</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>tmp12</t>
   </si>
 </sst>
 </file>
@@ -154,7 +179,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -242,11 +267,73 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -287,6 +374,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +709,7 @@
   <dimension ref="E4:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +784,9 @@
       <c r="I8" s="4">
         <v>18</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="10" t="s">
+        <v>37</v>
+      </c>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
     </row>
@@ -699,7 +806,9 @@
       <c r="I9" s="4">
         <v>19</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="10" t="s">
+        <v>38</v>
+      </c>
       <c r="K9" s="5"/>
       <c r="L9" s="6"/>
     </row>
@@ -865,7 +974,9 @@
       <c r="I18" s="4">
         <v>28</v>
       </c>
-      <c r="J18" s="10"/>
+      <c r="J18" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="K18" s="5"/>
       <c r="L18" s="6"/>
     </row>
@@ -948,6 +1059,64 @@
     <row r="28" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E28" s="1"/>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="25"/>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="25"/>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="25"/>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="25"/>
+    </row>
+    <row r="10" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="27"/>
+    </row>
+    <row r="11" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated reg convention excel
</commit_message>
<xml_diff>
--- a/ref/reg convention.xlsx
+++ b/ref/reg convention.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27106"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter Lee\Desktop\350 Final proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityasrinivasan/Documents/GitHub/fpga-logo/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10344"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27900" windowHeight="15700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DMEM state " sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -54,12 +60,6 @@
     <t>West</t>
   </si>
   <si>
-    <t>arg0</t>
-  </si>
-  <si>
-    <t>arg1</t>
-  </si>
-  <si>
     <t>tmp0</t>
   </si>
   <si>
@@ -117,9 +117,6 @@
     <t>tmp11</t>
   </si>
   <si>
-    <t>pen down/up</t>
-  </si>
-  <si>
     <t>DMEM stack ptr</t>
   </si>
   <si>
@@ -144,15 +141,24 @@
     <t>Command</t>
   </si>
   <si>
-    <t>tmp12</t>
+    <t>arg1 (mult arg)</t>
+  </si>
+  <si>
+    <t>arg2 (mult arg)</t>
+  </si>
+  <si>
+    <t>arg0 (command arg)</t>
+  </si>
+  <si>
+    <t>DMEM state pointer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -335,13 +341,13 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -708,19 +714,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E4" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="5:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="E6" s="2">
         <v>0</v>
       </c>
@@ -731,7 +741,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I6" s="2">
         <v>16</v>
@@ -741,10 +751,10 @@
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E7" s="4">
         <v>1</v>
       </c>
@@ -755,20 +765,20 @@
         <v>6</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I7" s="4">
         <v>17</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E8" s="4">
         <v>2</v>
       </c>
@@ -779,18 +789,18 @@
         <v>7</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I8" s="4">
         <v>18</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
     </row>
-    <row r="9" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E9" s="4">
         <v>3</v>
       </c>
@@ -801,23 +811,23 @@
         <v>8</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I9" s="4">
         <v>19</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="6"/>
     </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E10" s="4">
         <v>4</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="17"/>
@@ -825,17 +835,17 @@
         <v>20</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E11" s="4">
         <v>5</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
@@ -843,17 +853,17 @@
         <v>21</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E12" s="4">
         <v>6</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
@@ -861,17 +871,17 @@
         <v>22</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E13" s="4">
         <v>7</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
@@ -879,17 +889,17 @@
         <v>23</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E14" s="4">
         <v>8</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
@@ -897,17 +907,17 @@
         <v>24</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E15" s="4">
         <v>9</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="6"/>
@@ -915,12 +925,12 @@
         <v>25</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E16" s="4">
         <v>10</v>
       </c>
@@ -929,18 +939,18 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I16" s="4">
         <v>26</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E17" s="4">
         <v>11</v>
       </c>
@@ -949,18 +959,18 @@
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I17" s="4">
         <v>27</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E18" s="4">
         <v>12</v>
       </c>
@@ -969,38 +979,38 @@
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I18" s="4">
         <v>28</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K18" s="5"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E19" s="4">
         <v>13</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I19" s="4">
         <v>29</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="K19" s="5"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E20" s="4">
         <v>14</v>
       </c>
@@ -1009,18 +1019,18 @@
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I20" s="4">
         <v>30</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="21"/>
     </row>
-    <row r="21" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E21" s="7">
         <v>15</v>
       </c>
@@ -1029,7 +1039,7 @@
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I21" s="7">
         <v>31</v>
@@ -1040,23 +1050,23 @@
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:12" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:12" x14ac:dyDescent="0.2">
       <c r="E28" s="1"/>
     </row>
   </sheetData>
@@ -1072,51 +1082,51 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C5" s="22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D5" s="23"/>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="25"/>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7" s="24" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="25"/>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C8" s="24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8" s="25"/>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C9" s="24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="25"/>
     </row>
-    <row r="10" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10" s="27"/>
     </row>
-    <row r="11" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="3:4" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Free , ,  and use  instead
</commit_message>
<xml_diff>
--- a/ref/reg convention.xlsx
+++ b/ref/reg convention.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27106"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityasrinivasan/Documents/GitHub/fpga-logo/ref/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hunter Lee\Documents\GitHub\fpga-logo\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27900" windowHeight="15700"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="27900" windowHeight="15696"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="DMEM state " sheetId="2" r:id="rId2"/>
+    <sheet name="DMEM layout" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>JR</t>
   </si>
@@ -151,14 +152,47 @@
   </si>
   <si>
     <t>DMEM state pointer</t>
+  </si>
+  <si>
+    <t>Color code: 0, 1, 2, 3, etc…</t>
+  </si>
+  <si>
+    <t>Orientation Code</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Const</t>
+  </si>
+  <si>
+    <t>Function pointer</t>
+  </si>
+  <si>
+    <t>Turtle Images * 4</t>
+  </si>
+  <si>
+    <t>States</t>
+  </si>
+  <si>
+    <t>*Memory grows downward</t>
+  </si>
+  <si>
+    <t>Addr</t>
+  </si>
+  <si>
+    <t>reserved temp reg</t>
+  </si>
+  <si>
+    <t>Direction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -185,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -335,19 +369,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -397,6 +449,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -712,25 +781,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E4:L28"/>
+  <dimension ref="E4:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E4" s="20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="5:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="5:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="5:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M5" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="N5" s="28"/>
+      <c r="O5" s="29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="5:15" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="E6" s="2">
         <v>0</v>
       </c>
@@ -738,11 +818,9 @@
         <v>0</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>14</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="H6" s="15"/>
       <c r="I6" s="2">
         <v>16</v>
       </c>
@@ -753,20 +831,27 @@
       <c r="L6" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E7" s="4">
         <v>1</v>
       </c>
-      <c r="F7" s="12">
-        <v>1</v>
+      <c r="F7" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>15</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H7" s="17"/>
       <c r="I7" s="4">
         <v>17</v>
       </c>
@@ -777,20 +862,23 @@
       <c r="L7" s="17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="F8" s="12">
-        <v>2</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
       <c r="I8" s="4">
         <v>18</v>
       </c>
@@ -799,20 +887,23 @@
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="F9" s="13">
-        <v>3</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>17</v>
-      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17"/>
       <c r="I9" s="4">
         <v>19</v>
       </c>
@@ -821,8 +912,17 @@
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E10" s="4">
         <v>4</v>
       </c>
@@ -840,7 +940,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E11" s="4">
         <v>5</v>
       </c>
@@ -858,7 +958,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="6"/>
     </row>
-    <row r="12" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E12" s="4">
         <v>6</v>
       </c>
@@ -876,7 +976,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="6"/>
     </row>
-    <row r="13" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E13" s="4">
         <v>7</v>
       </c>
@@ -894,7 +994,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="6"/>
     </row>
-    <row r="14" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E14" s="4">
         <v>8</v>
       </c>
@@ -912,7 +1012,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="6"/>
     </row>
-    <row r="15" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E15" s="4">
         <v>9</v>
       </c>
@@ -930,7 +1030,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="6"/>
     </row>
-    <row r="16" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E16" s="4">
         <v>10</v>
       </c>
@@ -950,7 +1050,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E17" s="4">
         <v>11</v>
       </c>
@@ -970,7 +1070,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E18" s="4">
         <v>12</v>
       </c>
@@ -990,7 +1090,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="6"/>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E19" s="4">
         <v>13</v>
       </c>
@@ -1010,7 +1110,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="6"/>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E20" s="4">
         <v>14</v>
       </c>
@@ -1030,7 +1130,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="21"/>
     </row>
-    <row r="21" spans="5:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E21" s="7">
         <v>15</v>
       </c>
@@ -1050,23 +1150,23 @@
       <c r="K21" s="8"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="5:12" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E28" s="1"/>
     </row>
   </sheetData>
@@ -1079,54 +1179,197 @@
   <dimension ref="C3:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="3:4" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C5" s="22" t="s">
         <v>30</v>
       </c>
       <c r="D5" s="23"/>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" s="24" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="25"/>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C7" s="24" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="25"/>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C8" s="24" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="25"/>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9" s="24" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="25"/>
     </row>
-    <row r="10" spans="3:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="27"/>
     </row>
-    <row r="11" spans="3:4" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C5" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="34"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="33"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="34"/>
+      <c r="F6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="33"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="34"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="33"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="34"/>
+      <c r="F8">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="33"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="34"/>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="33"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="34"/>
+      <c r="F10">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="33"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="34"/>
+    </row>
+    <row r="12" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37"/>
+    </row>
+    <row r="13" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="34"/>
+      <c r="F13">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="33"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="34"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="33"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="34"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="33"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="34"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="33"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="34"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="33"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="34"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="33"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="34"/>
+    </row>
+    <row r="20" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="33"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="34"/>
+    </row>
+    <row r="21" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37"/>
+    </row>
+    <row r="23" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modify DMEM state convention
</commit_message>
<xml_diff>
--- a/ref/reg convention.xlsx
+++ b/ref/reg convention.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="27900" windowHeight="15696"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="27900" windowHeight="15696" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>JR</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Direction</t>
+  </si>
+  <si>
+    <t>penup/down</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -466,6 +469,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -783,7 +789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1176,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:D11"/>
+  <dimension ref="C3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1220,13 +1226,19 @@
       </c>
       <c r="D9" s="25"/>
     </row>
-    <row r="10" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="26" t="s">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="25"/>
+    </row>
+    <row r="11" spans="3:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="27"/>
-    </row>
-    <row r="11" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="D11" s="27"/>
+    </row>
+    <row r="12" spans="3:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add layout convention 2
</commit_message>
<xml_diff>
--- a/ref/reg convention.xlsx
+++ b/ref/reg convention.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="27900" windowHeight="15696"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="27900" windowHeight="15696" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>JR</t>
   </si>
@@ -166,15 +166,6 @@
     <t>Const</t>
   </si>
   <si>
-    <t>Function pointer</t>
-  </si>
-  <si>
-    <t>Turtle Images * 4</t>
-  </si>
-  <si>
-    <t>States</t>
-  </si>
-  <si>
     <t>*Memory grows downward</t>
   </si>
   <si>
@@ -200,6 +191,18 @@
   </si>
   <si>
     <t>1: down</t>
+  </si>
+  <si>
+    <t>state ptr</t>
+  </si>
+  <si>
+    <t>Turtle Images * 2</t>
+  </si>
+  <si>
+    <t>function ptr</t>
+  </si>
+  <si>
+    <t>Letters</t>
   </si>
 </sst>
 </file>
@@ -234,7 +237,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -402,11 +405,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -482,6 +522,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,7 +841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="150" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -861,10 +904,10 @@
         <v>1</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="4">
@@ -892,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="15"/>
@@ -919,13 +962,13 @@
         <v>3</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I9" s="4">
         <v>19</v>
@@ -1245,7 +1288,7 @@
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" s="37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D10" s="23"/>
     </row>
@@ -1265,15 +1308,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1284,12 +1327,12 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="31" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="32"/>
@@ -1302,13 +1345,15 @@
         <v>900</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C7" s="31"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="32"/>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="31"/>
+    <row r="7" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="33"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="35"/>
+    </row>
+    <row r="8" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="31" t="s">
+        <v>53</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="32"/>
       <c r="F8">
@@ -1328,19 +1373,24 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="31"/>
       <c r="D11" s="5"/>
       <c r="E11" s="32"/>
     </row>
-    <row r="12" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="33"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="35"/>
+    <row r="12" spans="3:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
+      <c r="F12">
+        <v>3500</v>
+      </c>
     </row>
     <row r="13" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C13" s="31" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="32"/>
@@ -1378,17 +1428,15 @@
       <c r="D19" s="5"/>
       <c r="E19" s="32"/>
     </row>
-    <row r="20" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="31"/>
       <c r="D20" s="5"/>
       <c r="E20" s="32"/>
     </row>
-    <row r="21" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="29"/>
-      <c r="E21" s="30"/>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="31"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="32"/>
       <c r="F21">
         <v>4000</v>
       </c>

</xml_diff>